<commit_message>
Add results for 2022-02-21
</commit_message>
<xml_diff>
--- a/data/2022-02-21/SCW Weekly Comp 2022-02-21 (Responses).xlsx
+++ b/data/2022-02-21/SCW Weekly Comp 2022-02-21 (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="199">
   <si>
     <t>Timestamp</t>
   </si>
@@ -581,6 +581,33 @@
   </si>
   <si>
     <t>Meh</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/627504321814800/?post_id=635575847674314&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>4:07.45</t>
+  </si>
+  <si>
+    <t>4:15.37</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/283377510532834/?post_id=291748173029101&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>Eric Dodson</t>
+  </si>
+  <si>
+    <t>2021DODS01</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/283377510532834/?post_id=291856813018237&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/283377510532834/?post_id=291865509684034&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/509549287201075/?post_id=518753962947274&amp;view=permalink</t>
   </si>
 </sst>
 </file>
@@ -605,12 +632,18 @@
       <color rgb="FF0000FF"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -619,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -634,6 +667,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1499,7 +1535,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>44617.49460528935</v>
+        <v>44617.55181474537</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>26</v>
@@ -1513,6 +1549,9 @@
       <c r="F10" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="G10" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="BH10" s="3">
         <v>12.68</v>
       </c>
@@ -1537,48 +1576,42 @@
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>44617.55181474537</v>
+        <v>44618.06328538194</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="BH11" s="3">
-        <v>12.68</v>
-      </c>
-      <c r="BI11" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="BJ11" s="3">
-        <v>11.2</v>
-      </c>
-      <c r="BK11" s="3">
-        <v>11.25</v>
-      </c>
-      <c r="BL11" s="3">
-        <v>11.55</v>
-      </c>
-      <c r="BM11" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="BN11" s="3">
-        <v>11.33</v>
+        <v>48</v>
+      </c>
+      <c r="CT11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="CU11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="CV11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="CW11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="CX11" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>44618.06328538194</v>
+        <v>44618.06406827546</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>19</v>
@@ -1590,65 +1623,68 @@
         <v>21</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="CT12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="CO12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="CU12" s="3" t="s">
+      <c r="CP12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="CQ12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="CV12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="CW12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="CX12" s="3" t="s">
+      <c r="CR12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="CS12" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
-        <v>44618.06406827546</v>
+        <v>44618.24775260416</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="CO13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="CP13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="CQ13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="CR13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="CS13" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="H13" s="3">
+        <v>11.56</v>
+      </c>
+      <c r="I13" s="3">
+        <v>10.63</v>
+      </c>
+      <c r="J13" s="3">
+        <v>11.65</v>
+      </c>
+      <c r="K13" s="3">
+        <v>24.36</v>
+      </c>
+      <c r="L13" s="3">
+        <v>18.64</v>
+      </c>
+      <c r="M13" s="3">
+        <v>10.63</v>
+      </c>
+      <c r="N13" s="3">
+        <v>13.95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
-        <v>44618.24775260416</v>
+        <v>44618.2547194213</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>54</v>
@@ -1657,36 +1693,36 @@
         <v>20</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="3">
-        <v>11.56</v>
-      </c>
-      <c r="I14" s="3">
-        <v>10.63</v>
-      </c>
-      <c r="J14" s="3">
-        <v>11.65</v>
-      </c>
-      <c r="K14" s="3">
-        <v>24.36</v>
-      </c>
-      <c r="L14" s="3">
-        <v>18.64</v>
-      </c>
-      <c r="M14" s="3">
-        <v>10.63</v>
-      </c>
-      <c r="N14" s="3">
-        <v>13.95</v>
+        <v>56</v>
+      </c>
+      <c r="BH14" s="3">
+        <v>24.4</v>
+      </c>
+      <c r="BI14" s="3">
+        <v>19.76</v>
+      </c>
+      <c r="BJ14" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="BK14" s="3">
+        <v>16.03</v>
+      </c>
+      <c r="BL14" s="3">
+        <v>16.02</v>
+      </c>
+      <c r="BM14" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="BN14" s="3">
+        <v>17.27</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
-        <v>44618.2547194213</v>
+        <v>44618.2559727662</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>54</v>
@@ -1695,36 +1731,36 @@
         <v>20</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="BH15" s="3">
-        <v>24.4</v>
-      </c>
-      <c r="BI15" s="3">
-        <v>19.76</v>
-      </c>
-      <c r="BJ15" s="3">
-        <v>14.8</v>
-      </c>
-      <c r="BK15" s="3">
-        <v>16.03</v>
-      </c>
-      <c r="BL15" s="3">
-        <v>16.02</v>
-      </c>
-      <c r="BM15" s="3">
-        <v>14.8</v>
-      </c>
-      <c r="BN15" s="3">
-        <v>17.27</v>
+        <v>58</v>
+      </c>
+      <c r="BO15" s="3">
+        <v>17.87</v>
+      </c>
+      <c r="BP15" s="3">
+        <v>21.03</v>
+      </c>
+      <c r="BQ15" s="3">
+        <v>23.67</v>
+      </c>
+      <c r="BR15" s="3">
+        <v>26.91</v>
+      </c>
+      <c r="BS15" s="3">
+        <v>19.64</v>
+      </c>
+      <c r="BT15" s="3">
+        <v>17.87</v>
+      </c>
+      <c r="BU15" s="3">
+        <v>21.45</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
-        <v>44618.2559727662</v>
+        <v>44618.257078993054</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>54</v>
@@ -1733,36 +1769,36 @@
         <v>20</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="BO16" s="3">
-        <v>17.87</v>
-      </c>
-      <c r="BP16" s="3">
-        <v>21.03</v>
-      </c>
-      <c r="BQ16" s="3">
-        <v>23.67</v>
-      </c>
-      <c r="BR16" s="3">
-        <v>26.91</v>
-      </c>
-      <c r="BS16" s="3">
-        <v>19.64</v>
-      </c>
-      <c r="BT16" s="3">
-        <v>17.87</v>
-      </c>
-      <c r="BU16" s="3">
-        <v>21.45</v>
+        <v>60</v>
+      </c>
+      <c r="BV16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="BW16" s="3">
+        <v>59.32</v>
+      </c>
+      <c r="BX16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="BY16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="BZ16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="CA16" s="3">
+        <v>59.32</v>
+      </c>
+      <c r="CB16" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
-        <v>44618.257078993054</v>
+        <v>44618.258144050924</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>54</v>
@@ -1771,36 +1807,36 @@
         <v>20</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="BV17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="BW17" s="3">
-        <v>59.32</v>
-      </c>
-      <c r="BX17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="BY17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BZ17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="CA17" s="3">
-        <v>59.32</v>
-      </c>
-      <c r="CB17" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="O17" s="3">
+        <v>29.6</v>
+      </c>
+      <c r="P17" s="3">
+        <v>24.25</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>23.0</v>
+      </c>
+      <c r="R17" s="3">
+        <v>24.98</v>
+      </c>
+      <c r="S17" s="3">
+        <v>18.76</v>
+      </c>
+      <c r="T17" s="3">
+        <v>18.76</v>
+      </c>
+      <c r="U17" s="3">
+        <v>24.08</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
-        <v>44618.258144050924</v>
+        <v>44618.259770324075</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>54</v>
@@ -1809,36 +1845,36 @@
         <v>20</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="O18" s="3">
-        <v>29.6</v>
-      </c>
-      <c r="P18" s="3">
-        <v>24.25</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="R18" s="3">
-        <v>24.98</v>
-      </c>
-      <c r="S18" s="3">
-        <v>18.76</v>
-      </c>
-      <c r="T18" s="3">
-        <v>18.76</v>
-      </c>
-      <c r="U18" s="3">
-        <v>24.08</v>
+        <v>67</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
-        <v>44618.259770324075</v>
+        <v>44618.261064652776</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>54</v>
@@ -1847,74 +1883,77 @@
         <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="V19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="W19" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="X19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB19" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="AC19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI19" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
-        <v>44618.261064652776</v>
+        <v>44618.92397506944</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD20" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE20" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF20" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG20" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH20" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI20" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="BO20" s="3">
+        <v>29.64</v>
+      </c>
+      <c r="BP20" s="3">
+        <v>37.79</v>
+      </c>
+      <c r="BQ20" s="3">
+        <v>25.32</v>
+      </c>
+      <c r="BR20" s="3">
+        <v>25.32</v>
+      </c>
+      <c r="BS20" s="3">
+        <v>15.41</v>
+      </c>
+      <c r="BT20" s="3">
+        <v>15.41</v>
+      </c>
+      <c r="BU20" s="3">
+        <v>26.76</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
-        <v>44618.92397506944</v>
+        <v>44618.92557690972</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>82</v>
@@ -1926,36 +1965,36 @@
         <v>83</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="BO21" s="3">
-        <v>29.64</v>
-      </c>
-      <c r="BP21" s="3">
-        <v>37.79</v>
-      </c>
-      <c r="BQ21" s="3">
-        <v>25.32</v>
-      </c>
-      <c r="BR21" s="3">
-        <v>25.32</v>
-      </c>
-      <c r="BS21" s="3">
-        <v>15.41</v>
-      </c>
-      <c r="BT21" s="3">
-        <v>15.41</v>
-      </c>
-      <c r="BU21" s="3">
-        <v>26.76</v>
+        <v>85</v>
+      </c>
+      <c r="BH21" s="3">
+        <v>24.84</v>
+      </c>
+      <c r="BI21" s="3">
+        <v>18.02</v>
+      </c>
+      <c r="BJ21" s="3">
+        <v>24.03</v>
+      </c>
+      <c r="BK21" s="3">
+        <v>22.47</v>
+      </c>
+      <c r="BL21" s="3">
+        <v>26.39</v>
+      </c>
+      <c r="BM21" s="3">
+        <v>18.02</v>
+      </c>
+      <c r="BN21" s="3">
+        <v>23.78</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
-        <v>44618.92557690972</v>
+        <v>44619.582967442126</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>82</v>
@@ -1967,36 +2006,36 @@
         <v>83</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="BH22" s="3">
-        <v>24.84</v>
-      </c>
-      <c r="BI22" s="3">
-        <v>18.02</v>
-      </c>
-      <c r="BJ22" s="3">
-        <v>24.03</v>
-      </c>
-      <c r="BK22" s="3">
-        <v>22.47</v>
-      </c>
-      <c r="BL22" s="3">
-        <v>26.39</v>
-      </c>
-      <c r="BM22" s="3">
-        <v>18.02</v>
-      </c>
-      <c r="BN22" s="3">
-        <v>23.78</v>
+        <v>86</v>
+      </c>
+      <c r="BV22" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BW22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="BX22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BY22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="BZ22" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="CA22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="CB22" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
-        <v>44619.582967442126</v>
+        <v>44619.58474568287</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>82</v>
@@ -2008,115 +2047,115 @@
         <v>83</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="BV23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BW23" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="BX23" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="BY23" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BZ23" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="CA23" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="CB23" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="CC23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="CD23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="CE23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="CF23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="CG23" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="CH23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="CI23" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
-        <v>44619.58474568287</v>
+        <v>44619.64570527778</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="CC24" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="CD24" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="CE24" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="CF24" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="CG24" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="CH24" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="CI24" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="O24" s="3">
+        <v>30.17</v>
+      </c>
+      <c r="P24" s="3">
+        <v>27.83</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>30.88</v>
+      </c>
+      <c r="R24" s="3">
+        <v>33.52</v>
+      </c>
+      <c r="S24" s="3">
+        <v>29.83</v>
+      </c>
+      <c r="T24" s="3">
+        <v>27.83</v>
+      </c>
+      <c r="U24" s="3">
+        <v>30.29</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
-        <v>44619.64570527778</v>
+        <v>44619.692299965274</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="O25" s="3">
-        <v>30.17</v>
+        <v>19.35</v>
       </c>
       <c r="P25" s="3">
-        <v>27.83</v>
+        <v>16.81</v>
       </c>
       <c r="Q25" s="3">
-        <v>30.88</v>
+        <v>22.07</v>
       </c>
       <c r="R25" s="3">
-        <v>33.52</v>
+        <v>17.25</v>
       </c>
       <c r="S25" s="3">
-        <v>29.83</v>
+        <v>19.82</v>
       </c>
       <c r="T25" s="3">
-        <v>27.83</v>
+        <v>16.81</v>
       </c>
       <c r="U25" s="3">
-        <v>30.29</v>
+        <v>18.81</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
-        <v>44619.692299965274</v>
+        <v>44619.69375133102</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>101</v>
@@ -2128,36 +2167,36 @@
         <v>102</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="O26" s="3">
-        <v>19.35</v>
-      </c>
-      <c r="P26" s="3">
-        <v>16.81</v>
-      </c>
-      <c r="Q26" s="3">
-        <v>22.07</v>
-      </c>
-      <c r="R26" s="3">
-        <v>17.25</v>
-      </c>
-      <c r="S26" s="3">
-        <v>19.82</v>
-      </c>
-      <c r="T26" s="3">
-        <v>16.81</v>
-      </c>
-      <c r="U26" s="3">
-        <v>18.81</v>
+        <v>104</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z26" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB26" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
-        <v>44619.69375133102</v>
+        <v>44619.69478024305</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>101</v>
@@ -2169,36 +2208,36 @@
         <v>102</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="V27" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="W27" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="X27" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y27" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z27" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA27" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AB27" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="AC27" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE27" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF27" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG27" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH27" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI27" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2">
-        <v>44619.69478024305</v>
+        <v>44619.69748721065</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>101</v>
@@ -2210,36 +2249,30 @@
         <v>102</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC28" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AE28" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF28" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG28" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH28" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AI28" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
+      </c>
+      <c r="AJ28" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK28" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL28" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM28" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AN28" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
-        <v>44619.69748721065</v>
+        <v>44619.698094363426</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>101</v>
@@ -2251,109 +2284,115 @@
         <v>102</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AJ29" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK29" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL29" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="AM29" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="AN29" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="AO29" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AP29" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AQ29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AR29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AS29" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
-        <v>44619.698094363426</v>
+        <v>44619.85386545139</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AO30" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="AP30" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ30" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AR30" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AS30" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
+      </c>
+      <c r="O30" s="3">
+        <v>24.08</v>
+      </c>
+      <c r="P30" s="3">
+        <v>31.99</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>22.19</v>
+      </c>
+      <c r="R30" s="3">
+        <v>28.38</v>
+      </c>
+      <c r="S30" s="3">
+        <v>23.33</v>
+      </c>
+      <c r="T30" s="3">
+        <v>22.19</v>
+      </c>
+      <c r="U30" s="3">
+        <v>25.26</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
-        <v>44619.85386545139</v>
+        <v>44621.92404084491</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>131</v>
+        <v>31</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="O31" s="3">
-        <v>24.08</v>
-      </c>
-      <c r="P31" s="3">
-        <v>31.99</v>
-      </c>
-      <c r="Q31" s="3">
-        <v>22.19</v>
-      </c>
-      <c r="R31" s="3">
-        <v>28.38</v>
-      </c>
-      <c r="S31" s="3">
-        <v>23.33</v>
-      </c>
-      <c r="T31" s="3">
-        <v>22.19</v>
-      </c>
-      <c r="U31" s="3">
-        <v>25.26</v>
+        <v>136</v>
+      </c>
+      <c r="CC31" s="3">
+        <v>8.84</v>
+      </c>
+      <c r="CD31" s="3">
+        <v>6.65</v>
+      </c>
+      <c r="CE31" s="3">
+        <v>6.66</v>
+      </c>
+      <c r="CF31" s="3">
+        <v>7.89</v>
+      </c>
+      <c r="CG31" s="3">
+        <v>8.18</v>
+      </c>
+      <c r="CH31" s="3">
+        <v>6.65</v>
+      </c>
+      <c r="CI31" s="3">
+        <v>7.58</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
-        <v>44621.92404084491</v>
+        <v>44621.92956532407</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>31</v>
@@ -2362,77 +2401,77 @@
         <v>135</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="CC32" s="3">
-        <v>8.84</v>
-      </c>
-      <c r="CD32" s="3">
-        <v>6.65</v>
-      </c>
-      <c r="CE32" s="3">
-        <v>6.66</v>
-      </c>
-      <c r="CF32" s="3">
-        <v>7.89</v>
-      </c>
-      <c r="CG32" s="3">
-        <v>8.18</v>
-      </c>
-      <c r="CH32" s="3">
-        <v>6.65</v>
-      </c>
-      <c r="CI32" s="3">
-        <v>7.58</v>
+        <v>138</v>
+      </c>
+      <c r="O32" s="3">
+        <v>15.53</v>
+      </c>
+      <c r="P32" s="3">
+        <v>17.12</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>22.42</v>
+      </c>
+      <c r="R32" s="3">
+        <v>16.4</v>
+      </c>
+      <c r="S32" s="3">
+        <v>18.23</v>
+      </c>
+      <c r="T32" s="3">
+        <v>15.53</v>
+      </c>
+      <c r="U32" s="3">
+        <v>17.25</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
-        <v>44621.92956532407</v>
+        <v>44623.95117335649</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="O33" s="3">
-        <v>15.53</v>
-      </c>
-      <c r="P33" s="3">
-        <v>17.12</v>
-      </c>
-      <c r="Q33" s="3">
-        <v>22.42</v>
-      </c>
-      <c r="R33" s="3">
-        <v>16.4</v>
-      </c>
-      <c r="S33" s="3">
-        <v>18.23</v>
-      </c>
-      <c r="T33" s="3">
-        <v>15.53</v>
-      </c>
-      <c r="U33" s="3">
-        <v>17.25</v>
+        <v>139</v>
+      </c>
+      <c r="CC33" s="3">
+        <v>14.47</v>
+      </c>
+      <c r="CD33" s="3">
+        <v>11.02</v>
+      </c>
+      <c r="CE33" s="3">
+        <v>13.65</v>
+      </c>
+      <c r="CF33" s="3">
+        <v>10.94</v>
+      </c>
+      <c r="CG33" s="3">
+        <v>12.95</v>
+      </c>
+      <c r="CH33" s="3">
+        <v>10.94</v>
+      </c>
+      <c r="CI33" s="3">
+        <v>12.54</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
-        <v>44623.95117335649</v>
+        <v>44624.75456434028</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>130</v>
@@ -2444,36 +2483,36 @@
         <v>132</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="CC34" s="3">
-        <v>14.47</v>
-      </c>
-      <c r="CD34" s="3">
-        <v>11.02</v>
-      </c>
-      <c r="CE34" s="3">
-        <v>13.65</v>
-      </c>
-      <c r="CF34" s="3">
-        <v>10.94</v>
-      </c>
-      <c r="CG34" s="3">
-        <v>12.95</v>
-      </c>
-      <c r="CH34" s="3">
-        <v>10.94</v>
-      </c>
-      <c r="CI34" s="3">
-        <v>12.54</v>
+        <v>140</v>
+      </c>
+      <c r="BO34" s="3">
+        <v>12.58</v>
+      </c>
+      <c r="BP34" s="3">
+        <v>13.68</v>
+      </c>
+      <c r="BQ34" s="3">
+        <v>15.35</v>
+      </c>
+      <c r="BR34" s="3">
+        <v>35.94</v>
+      </c>
+      <c r="BS34" s="3">
+        <v>16.21</v>
+      </c>
+      <c r="BT34" s="3">
+        <v>12.58</v>
+      </c>
+      <c r="BU34" s="3">
+        <v>15.08</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2">
-        <v>44624.75456434028</v>
+        <v>44624.75526630787</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>130</v>
@@ -2485,36 +2524,36 @@
         <v>132</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="BO35" s="3">
-        <v>12.58</v>
-      </c>
-      <c r="BP35" s="3">
-        <v>13.68</v>
-      </c>
-      <c r="BQ35" s="3">
-        <v>15.35</v>
-      </c>
-      <c r="BR35" s="3">
-        <v>35.94</v>
-      </c>
-      <c r="BS35" s="3">
-        <v>16.21</v>
-      </c>
-      <c r="BT35" s="3">
-        <v>12.58</v>
-      </c>
-      <c r="BU35" s="3">
-        <v>15.08</v>
+        <v>141</v>
+      </c>
+      <c r="BH35" s="3">
+        <v>12.09</v>
+      </c>
+      <c r="BI35" s="3">
+        <v>13.47</v>
+      </c>
+      <c r="BJ35" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="BK35" s="3">
+        <v>13.64</v>
+      </c>
+      <c r="BL35" s="3">
+        <v>19.57</v>
+      </c>
+      <c r="BM35" s="3">
+        <v>5.65</v>
+      </c>
+      <c r="BN35" s="3">
+        <v>13.07</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
-        <v>44624.75526630787</v>
+        <v>44624.75597179398</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>130</v>
@@ -2526,153 +2565,153 @@
         <v>132</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="BH36" s="3">
-        <v>12.09</v>
-      </c>
-      <c r="BI36" s="3">
-        <v>13.47</v>
-      </c>
-      <c r="BJ36" s="3">
-        <v>5.65</v>
-      </c>
-      <c r="BK36" s="3">
-        <v>13.64</v>
-      </c>
-      <c r="BL36" s="3">
-        <v>19.57</v>
-      </c>
-      <c r="BM36" s="3">
-        <v>5.65</v>
-      </c>
-      <c r="BN36" s="3">
-        <v>13.07</v>
+        <v>142</v>
+      </c>
+      <c r="H36" s="3">
+        <v>9.02</v>
+      </c>
+      <c r="I36" s="3">
+        <v>8.66</v>
+      </c>
+      <c r="J36" s="3">
+        <v>8.79</v>
+      </c>
+      <c r="K36" s="3">
+        <v>6.43</v>
+      </c>
+      <c r="L36" s="3">
+        <v>8.37</v>
+      </c>
+      <c r="M36" s="3">
+        <v>6.43</v>
+      </c>
+      <c r="N36" s="6">
+        <v>8.61</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
-        <v>44624.75597179398</v>
+        <v>44625.79181623843</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>132</v>
+        <v>31</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H37" s="3">
-        <v>9.02</v>
-      </c>
-      <c r="I37" s="3">
-        <v>8.66</v>
-      </c>
-      <c r="J37" s="3">
-        <v>8.79</v>
-      </c>
-      <c r="K37" s="3">
-        <v>6.43</v>
-      </c>
-      <c r="L37" s="3">
-        <v>8.37</v>
-      </c>
-      <c r="M37" s="3">
-        <v>6.43</v>
-      </c>
-      <c r="N37" s="3">
-        <v>8.37</v>
+        <v>144</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ37" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="AK37" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AL37" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM37" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AN37" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
-        <v>44625.79181623843</v>
+        <v>44626.237602152774</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>118</v>
+        <v>33</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="AJ38" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AK38" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="AL38" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="AM38" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="AN38" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
+      </c>
+      <c r="O38" s="3">
+        <v>19.31</v>
+      </c>
+      <c r="P38" s="3">
+        <v>17.59</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>18.03</v>
+      </c>
+      <c r="R38" s="3">
+        <v>19.51</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T38" s="3">
+        <v>17.59</v>
+      </c>
+      <c r="U38" s="3">
+        <v>18.95</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
-        <v>44626.237602152774</v>
+        <v>44626.65544349537</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="O39" s="3">
-        <v>19.31</v>
+        <v>19.56</v>
       </c>
       <c r="P39" s="3">
-        <v>17.59</v>
+        <v>15.32</v>
       </c>
       <c r="Q39" s="3">
-        <v>18.03</v>
+        <v>16.71</v>
       </c>
       <c r="R39" s="3">
-        <v>19.51</v>
-      </c>
-      <c r="S39" s="3" t="s">
-        <v>49</v>
+        <v>21.52</v>
+      </c>
+      <c r="S39" s="3">
+        <v>13.59</v>
       </c>
       <c r="T39" s="3">
-        <v>17.59</v>
+        <v>13.59</v>
       </c>
       <c r="U39" s="3">
-        <v>18.95</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
-        <v>44626.65544349537</v>
+        <v>44626.65617872685</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>153</v>
@@ -2684,71 +2723,71 @@
         <v>154</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="O40" s="3">
-        <v>19.56</v>
-      </c>
-      <c r="P40" s="3">
-        <v>15.32</v>
-      </c>
-      <c r="Q40" s="3">
-        <v>16.71</v>
-      </c>
-      <c r="R40" s="3">
-        <v>21.52</v>
-      </c>
-      <c r="S40" s="3">
-        <v>13.59</v>
-      </c>
-      <c r="T40" s="3">
-        <v>13.59</v>
-      </c>
-      <c r="U40" s="3">
-        <v>17.2</v>
+        <v>156</v>
+      </c>
+      <c r="CJ40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="CK40" s="3">
+        <v>35.0</v>
+      </c>
+      <c r="CL40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="CM40" s="3">
+        <v>35.0</v>
+      </c>
+      <c r="CN40" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
-        <v>44626.65617872685</v>
+        <v>44626.747432511576</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="CJ41" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="CK41" s="3">
-        <v>35.0</v>
-      </c>
-      <c r="CL41" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="CM41" s="3">
-        <v>35.0</v>
-      </c>
-      <c r="CN41" s="3" t="s">
-        <v>49</v>
+        <v>159</v>
+      </c>
+      <c r="BV41" s="3">
+        <v>23.82</v>
+      </c>
+      <c r="BW41" s="3">
+        <v>24.63</v>
+      </c>
+      <c r="BX41" s="3">
+        <v>16.28</v>
+      </c>
+      <c r="BY41" s="3">
+        <v>18.47</v>
+      </c>
+      <c r="BZ41" s="3">
+        <v>22.15</v>
+      </c>
+      <c r="CA41" s="3">
+        <v>16.28</v>
+      </c>
+      <c r="CB41" s="3">
+        <v>21.48</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
-        <v>44626.747432511576</v>
+        <v>44626.749046620374</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>157</v>
@@ -2760,36 +2799,36 @@
         <v>158</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="BV42" s="3">
-        <v>23.82</v>
-      </c>
-      <c r="BW42" s="3">
-        <v>24.63</v>
-      </c>
-      <c r="BX42" s="3">
-        <v>16.28</v>
-      </c>
-      <c r="BY42" s="3">
-        <v>18.47</v>
-      </c>
-      <c r="BZ42" s="3">
-        <v>22.15</v>
-      </c>
-      <c r="CA42" s="3">
-        <v>16.28</v>
-      </c>
-      <c r="CB42" s="3">
-        <v>21.48</v>
+      <c r="BH42" s="3">
+        <v>11.58</v>
+      </c>
+      <c r="BI42" s="3">
+        <v>13.19</v>
+      </c>
+      <c r="BJ42" s="3">
+        <v>17.34</v>
+      </c>
+      <c r="BK42" s="3">
+        <v>12.21</v>
+      </c>
+      <c r="BL42" s="3">
+        <v>10.19</v>
+      </c>
+      <c r="BM42" s="3">
+        <v>10.19</v>
+      </c>
+      <c r="BN42" s="3">
+        <v>12.33</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
-        <v>44626.749046620374</v>
+        <v>44626.75098078704</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>157</v>
@@ -2801,36 +2840,36 @@
         <v>158</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="BH43" s="3">
-        <v>11.58</v>
-      </c>
-      <c r="BI43" s="3">
-        <v>13.19</v>
-      </c>
-      <c r="BJ43" s="3">
-        <v>17.34</v>
-      </c>
-      <c r="BK43" s="3">
-        <v>12.21</v>
-      </c>
-      <c r="BL43" s="3">
-        <v>10.19</v>
-      </c>
-      <c r="BM43" s="3">
-        <v>10.19</v>
-      </c>
-      <c r="BN43" s="3">
-        <v>12.33</v>
+        <v>160</v>
+      </c>
+      <c r="H43" s="3">
+        <v>16.96</v>
+      </c>
+      <c r="I43" s="3">
+        <v>9.79</v>
+      </c>
+      <c r="J43" s="3">
+        <v>12.83</v>
+      </c>
+      <c r="K43" s="3">
+        <v>10.13</v>
+      </c>
+      <c r="L43" s="3">
+        <v>9.32</v>
+      </c>
+      <c r="M43" s="3">
+        <v>9.32</v>
+      </c>
+      <c r="N43" s="3">
+        <v>10.92</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2">
-        <v>44626.75098078704</v>
+        <v>44626.75234688657</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>157</v>
@@ -2842,36 +2881,36 @@
         <v>158</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="H44" s="3">
-        <v>16.96</v>
-      </c>
-      <c r="I44" s="3">
-        <v>9.79</v>
-      </c>
-      <c r="J44" s="3">
-        <v>12.83</v>
-      </c>
-      <c r="K44" s="3">
-        <v>10.13</v>
-      </c>
-      <c r="L44" s="3">
-        <v>9.32</v>
-      </c>
-      <c r="M44" s="3">
-        <v>9.32</v>
-      </c>
-      <c r="N44" s="3">
-        <v>10.92</v>
+      <c r="O44" s="3">
+        <v>24.22</v>
+      </c>
+      <c r="P44" s="3">
+        <v>27.16</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>27.25</v>
+      </c>
+      <c r="R44" s="3">
+        <v>27.34</v>
+      </c>
+      <c r="S44" s="3">
+        <v>25.94</v>
+      </c>
+      <c r="T44" s="3">
+        <v>24.22</v>
+      </c>
+      <c r="U44" s="3">
+        <v>26.78</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
-        <v>44626.75234688657</v>
+        <v>44626.75353460648</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>157</v>
@@ -2883,36 +2922,36 @@
         <v>158</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="O45" s="3">
-        <v>24.22</v>
-      </c>
-      <c r="P45" s="3">
-        <v>27.16</v>
-      </c>
-      <c r="Q45" s="3">
-        <v>27.25</v>
-      </c>
-      <c r="R45" s="3">
-        <v>27.34</v>
-      </c>
-      <c r="S45" s="3">
-        <v>25.94</v>
-      </c>
-      <c r="T45" s="3">
-        <v>24.22</v>
-      </c>
-      <c r="U45" s="3">
-        <v>26.78</v>
+        <v>161</v>
+      </c>
+      <c r="V45" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="W45" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="X45" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y45" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z45" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA45" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB45" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2">
-        <v>44626.75353460648</v>
+        <v>44626.75561982639</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>157</v>
@@ -2924,36 +2963,36 @@
         <v>158</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="V46" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="W46" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="X46" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="Y46" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z46" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AA46" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="AB46" s="3" t="s">
-        <v>167</v>
+      <c r="AC46" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD46" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE46" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF46" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG46" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH46" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="AI46" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2">
-        <v>44626.75561982639</v>
+        <v>44626.75642883102</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>157</v>
@@ -2965,71 +3004,71 @@
         <v>158</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="AC47" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="AD47" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE47" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="AF47" s="3" t="s">
+      <c r="AJ47" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="AK47" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AL47" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="AG47" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="AH47" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="AI47" s="3" t="s">
-        <v>172</v>
+      <c r="AM47" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AN47" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2">
-        <v>44626.75642883102</v>
+        <v>44626.77255890046</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>118</v>
+        <v>28</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="AJ48" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="AK48" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AL48" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="AM48" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AN48" s="3" t="s">
-        <v>49</v>
+        <v>177</v>
+      </c>
+      <c r="H48" s="3">
+        <v>9.65</v>
+      </c>
+      <c r="I48" s="3">
+        <v>8.72</v>
+      </c>
+      <c r="J48" s="3">
+        <v>8.75</v>
+      </c>
+      <c r="K48" s="3">
+        <v>9.29</v>
+      </c>
+      <c r="L48" s="3">
+        <v>9.53</v>
+      </c>
+      <c r="M48" s="3">
+        <v>8.72</v>
+      </c>
+      <c r="N48" s="3">
+        <v>9.19</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2">
-        <v>44626.77255890046</v>
+        <v>44626.77377752315</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>175</v>
@@ -3041,36 +3080,36 @@
         <v>176</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H49" s="3">
-        <v>9.65</v>
-      </c>
-      <c r="I49" s="3">
-        <v>8.72</v>
-      </c>
-      <c r="J49" s="3">
-        <v>8.75</v>
-      </c>
-      <c r="K49" s="3">
-        <v>9.29</v>
-      </c>
-      <c r="L49" s="3">
-        <v>9.53</v>
-      </c>
-      <c r="M49" s="3">
-        <v>8.72</v>
-      </c>
-      <c r="N49" s="3">
-        <v>9.19</v>
+        <v>178</v>
+      </c>
+      <c r="O49" s="3">
+        <v>32.89</v>
+      </c>
+      <c r="P49" s="3">
+        <v>30.78</v>
+      </c>
+      <c r="Q49" s="3">
+        <v>30.13</v>
+      </c>
+      <c r="R49" s="3">
+        <v>28.09</v>
+      </c>
+      <c r="S49" s="3">
+        <v>33.95</v>
+      </c>
+      <c r="T49" s="3">
+        <v>28.09</v>
+      </c>
+      <c r="U49" s="3">
+        <v>31.27</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2">
-        <v>44626.77377752315</v>
+        <v>44626.77520741898</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>175</v>
@@ -3082,195 +3121,359 @@
         <v>176</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="O50" s="3">
-        <v>32.89</v>
-      </c>
-      <c r="P50" s="3">
-        <v>30.78</v>
-      </c>
-      <c r="Q50" s="3">
-        <v>30.13</v>
-      </c>
-      <c r="R50" s="3">
-        <v>28.09</v>
-      </c>
-      <c r="S50" s="3">
-        <v>33.95</v>
-      </c>
-      <c r="T50" s="3">
-        <v>28.09</v>
-      </c>
-      <c r="U50" s="3">
-        <v>31.27</v>
+        <v>179</v>
+      </c>
+      <c r="BV50" s="3">
+        <v>47.53</v>
+      </c>
+      <c r="BW50" s="3">
+        <v>55.31</v>
+      </c>
+      <c r="BX50" s="3">
+        <v>41.93</v>
+      </c>
+      <c r="BY50" s="3">
+        <v>37.95</v>
+      </c>
+      <c r="BZ50" s="3">
+        <v>51.84</v>
+      </c>
+      <c r="CA50" s="3">
+        <v>37.95</v>
+      </c>
+      <c r="CB50" s="3">
+        <v>47.1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2">
-        <v>44626.77520741898</v>
+        <v>44626.77522486111</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="BV51" s="3">
-        <v>47.53</v>
-      </c>
-      <c r="BW51" s="3">
-        <v>55.31</v>
-      </c>
-      <c r="BX51" s="3">
-        <v>41.93</v>
-      </c>
-      <c r="BY51" s="3">
-        <v>37.95</v>
-      </c>
-      <c r="BZ51" s="3">
-        <v>51.84</v>
-      </c>
-      <c r="CA51" s="3">
-        <v>37.95</v>
-      </c>
-      <c r="CB51" s="3">
-        <v>47.1</v>
+        <v>182</v>
+      </c>
+      <c r="O51" s="3">
+        <v>21.57</v>
+      </c>
+      <c r="P51" s="3">
+        <v>20.7</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>20.63</v>
+      </c>
+      <c r="R51" s="3">
+        <v>24.06</v>
+      </c>
+      <c r="S51" s="3">
+        <v>18.19</v>
+      </c>
+      <c r="T51" s="3">
+        <v>18.19</v>
+      </c>
+      <c r="U51" s="3">
+        <v>20.97</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2">
-        <v>44626.77522486111</v>
+        <v>44626.77659149306</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="O52" s="3">
-        <v>21.57</v>
-      </c>
-      <c r="P52" s="3">
-        <v>20.7</v>
-      </c>
-      <c r="Q52" s="3">
-        <v>20.63</v>
-      </c>
-      <c r="R52" s="3">
-        <v>24.06</v>
-      </c>
-      <c r="S52" s="3">
-        <v>18.19</v>
-      </c>
-      <c r="T52" s="3">
-        <v>18.19</v>
-      </c>
-      <c r="U52" s="3">
-        <v>20.97</v>
+        <v>183</v>
+      </c>
+      <c r="V52" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="W52" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="X52" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y52" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z52" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AA52" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB52" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
-        <v>44626.77659149306</v>
+        <v>44626.795240127314</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>176</v>
+        <v>31</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="V53" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="W53" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="X53" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="Y53" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="Z53" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="AA53" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB53" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="O53" s="3">
+        <v>19.9</v>
+      </c>
+      <c r="P53" s="3">
+        <v>27.18</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>22.86</v>
+      </c>
+      <c r="R53" s="3">
+        <v>21.82</v>
+      </c>
+      <c r="S53" s="3">
+        <v>23.77</v>
+      </c>
+      <c r="T53" s="3">
+        <v>19.9</v>
+      </c>
+      <c r="U53" s="3">
+        <v>22.82</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2">
-        <v>44626.795240127314</v>
+        <v>44626.93873034722</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="O54" s="3">
-        <v>19.9</v>
-      </c>
-      <c r="P54" s="3">
-        <v>27.18</v>
-      </c>
-      <c r="Q54" s="3">
-        <v>22.86</v>
-      </c>
-      <c r="R54" s="3">
-        <v>21.82</v>
-      </c>
-      <c r="S54" s="3">
-        <v>23.77</v>
-      </c>
-      <c r="T54" s="3">
-        <v>19.9</v>
-      </c>
-      <c r="U54" s="3">
-        <v>22.82</v>
+        <v>190</v>
+      </c>
+      <c r="AC54" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD54" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="AE54" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF54" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG54" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH54" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AI54" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2">
+        <v>44626.94781491898</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH55" s="3">
+        <v>28.79</v>
+      </c>
+      <c r="BI55" s="3">
+        <v>28.59</v>
+      </c>
+      <c r="BJ55" s="3">
+        <v>24.83</v>
+      </c>
+      <c r="BK55" s="3">
+        <v>54.65</v>
+      </c>
+      <c r="BL55" s="3">
+        <v>33.33</v>
+      </c>
+      <c r="BM55" s="3">
+        <v>24.83</v>
+      </c>
+      <c r="BN55" s="3">
+        <v>30.24</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2">
+        <v>44627.15459612268</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="BO56" s="3">
+        <v>9.23</v>
+      </c>
+      <c r="BP56" s="3">
+        <v>20.78</v>
+      </c>
+      <c r="BQ56" s="3">
+        <v>14.3</v>
+      </c>
+      <c r="BR56" s="3">
+        <v>13.53</v>
+      </c>
+      <c r="BS56" s="3">
+        <v>20.16</v>
+      </c>
+      <c r="BT56" s="3">
+        <v>9.23</v>
+      </c>
+      <c r="BU56" s="3">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2">
+        <v>44627.17136346065</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="BH57" s="3">
+        <v>15.03</v>
+      </c>
+      <c r="BI57" s="3">
+        <v>9.57</v>
+      </c>
+      <c r="BJ57" s="3">
+        <v>18.91</v>
+      </c>
+      <c r="BK57" s="3">
+        <v>15.49</v>
+      </c>
+      <c r="BL57" s="3">
+        <v>16.03</v>
+      </c>
+      <c r="BM57" s="3">
+        <v>9.57</v>
+      </c>
+      <c r="BN57" s="3">
+        <v>15.52</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2">
+        <v>44627.18814629629</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="H58" s="3">
+        <v>9.28</v>
+      </c>
+      <c r="I58" s="3">
+        <v>9.21</v>
+      </c>
+      <c r="J58" s="3">
+        <v>10.47</v>
+      </c>
+      <c r="K58" s="3">
+        <v>9.34</v>
+      </c>
+      <c r="L58" s="3">
+        <v>12.46</v>
+      </c>
+      <c r="M58" s="3">
+        <v>9.21</v>
+      </c>
+      <c r="N58" s="3">
+        <v>9.7</v>
       </c>
     </row>
   </sheetData>
@@ -3328,7 +3531,11 @@
     <hyperlink r:id="rId51" ref="F52"/>
     <hyperlink r:id="rId52" ref="F53"/>
     <hyperlink r:id="rId53" ref="F54"/>
+    <hyperlink r:id="rId54" ref="F55"/>
+    <hyperlink r:id="rId55" ref="F56"/>
+    <hyperlink r:id="rId56" ref="F57"/>
+    <hyperlink r:id="rId57" ref="F58"/>
   </hyperlinks>
-  <drawing r:id="rId54"/>
+  <drawing r:id="rId58"/>
 </worksheet>
 </file>
</xml_diff>